<commit_message>
finished chapter 3 part 8 of 12
</commit_message>
<xml_diff>
--- a/videos_Lengths.xlsx
+++ b/videos_Lengths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="135">
   <si>
     <t>Chapter 2 : JavaScript Language Fundamentals</t>
   </si>
@@ -418,13 +418,16 @@
   </si>
   <si>
     <t>total completed time so far</t>
+  </si>
+  <si>
+    <t>left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,8 +495,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +527,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -527,12 +548,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -549,14 +571,24 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="46" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="9" fillId="5" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF33"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -854,18 +886,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -1075,10 +1107,10 @@
       <c r="D3" s="12">
         <v>6.2615740740740748E-3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="17">
         <v>1.0636574074074074E-2</v>
       </c>
       <c r="I3" t="s">
@@ -1146,7 +1178,7 @@
       <c r="A4" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="12">
         <v>7.0023148148148154E-3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1155,10 +1187,10 @@
       <c r="D4" s="12">
         <v>8.8541666666666664E-3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="17">
         <v>9.8726851851851857E-3</v>
       </c>
       <c r="I4" t="s">
@@ -1229,10 +1261,10 @@
       <c r="D5" s="12">
         <v>7.1759259259259259E-3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="17">
         <v>1.0023148148148147E-2</v>
       </c>
       <c r="I5" t="s">
@@ -1303,10 +1335,10 @@
       <c r="D6" s="12">
         <v>8.1365740740740738E-3</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="16">
         <v>1.0983796296296297E-2</v>
       </c>
       <c r="I6" t="s">
@@ -1377,10 +1409,10 @@
       <c r="D7" s="12">
         <v>5.0810185185185186E-3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="16">
         <v>4.7106481481481478E-3</v>
       </c>
       <c r="I7" t="s">
@@ -1451,10 +1483,10 @@
       <c r="D8" s="12">
         <v>9.9652777777777778E-3</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="16">
         <v>7.6041666666666662E-3</v>
       </c>
       <c r="I8" t="s">
@@ -1507,10 +1539,10 @@
       <c r="D9" s="12">
         <v>7.0254629629629634E-3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="16">
         <v>7.083333333333333E-3</v>
       </c>
       <c r="I9" t="s">
@@ -1739,13 +1771,18 @@
       </c>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I19" s="10">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="I19" s="18">
         <v>9.9826388888888895E-2</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="19" t="s">
         <v>18</v>
       </c>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="7"/>
@@ -1822,6 +1859,13 @@
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="15">
+        <v>43784</v>
+      </c>
+      <c r="C24" s="2">
+        <f>SUM(G2:G9)</f>
+        <v>6.3182870370370375E-2</v>
+      </c>
       <c r="I24" s="10">
         <v>6.7789351851851851E-2</v>
       </c>
@@ -1831,6 +1875,13 @@
       <c r="X24" s="1"/>
     </row>
     <row r="25" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="2">
+        <f>G1-C24</f>
+        <v>3.6643518518518506E-2</v>
+      </c>
       <c r="I25" s="10">
         <v>5.5787037037037031E-2</v>
       </c>

</xml_diff>

<commit_message>
finished Chapter 4 partg 6: Loan Calculator Project
</commit_message>
<xml_diff>
--- a/videos_Lengths.xlsx
+++ b/videos_Lengths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="134">
   <si>
     <t>Chapter 2 : JavaScript Language Fundamentals</t>
   </si>
@@ -418,16 +418,13 @@
   </si>
   <si>
     <t>total completed time so far</t>
-  </si>
-  <si>
-    <t>left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,13 +492,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -529,12 +519,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FF66FF33"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FF33"/>
+        <fgColor rgb="FF336600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,11 +539,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -571,21 +561,24 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="46" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="46" fontId="9" fillId="5" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF336600"/>
+      <color rgb="FF66FF66"/>
+      <color rgb="FF339933"/>
+      <color rgb="FF008000"/>
       <color rgb="FF66FF33"/>
     </mruColors>
   </colors>
@@ -887,7 +880,7 @@
   <dimension ref="A1:AK36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +892,7 @@
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" customWidth="1"/>
@@ -1033,10 +1026,10 @@
       <c r="G2" s="12">
         <v>2.2685185185185182E-3</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="19">
         <v>1.1030092592592591E-2</v>
       </c>
       <c r="L2" t="s">
@@ -1113,10 +1106,10 @@
       <c r="G3" s="17">
         <v>1.0636574074074074E-2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="19">
         <v>9.7685185185185184E-3</v>
       </c>
       <c r="L3" t="s">
@@ -1193,10 +1186,10 @@
       <c r="G4" s="17">
         <v>9.8726851851851857E-3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="19">
         <v>7.6736111111111111E-3</v>
       </c>
       <c r="L4" t="s">
@@ -1267,10 +1260,10 @@
       <c r="G5" s="17">
         <v>1.0023148148148147E-2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="19">
         <v>1.0497685185185186E-2</v>
       </c>
       <c r="L5" t="s">
@@ -1583,10 +1576,10 @@
       <c r="D10" s="12">
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="16">
         <v>7.6851851851851847E-3</v>
       </c>
       <c r="I10" t="s">
@@ -1621,10 +1614,10 @@
       <c r="D11" s="12">
         <v>5.4398148148148149E-3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="16">
         <v>8.8310185185185176E-3</v>
       </c>
       <c r="I11" t="s">
@@ -1654,10 +1647,10 @@
       <c r="D12" s="12">
         <v>6.4120370370370364E-3</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="16">
         <v>9.5486111111111101E-3</v>
       </c>
       <c r="R12" t="s">
@@ -1680,10 +1673,10 @@
       <c r="D13" s="12">
         <v>1.3217592592592593E-2</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="19">
         <v>1.0578703703703703E-2</v>
       </c>
       <c r="R13" t="s">
@@ -1771,18 +1764,13 @@
       </c>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="I19" s="18">
+    <row r="19" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="I19" s="10">
         <v>9.9826388888888895E-2</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="7"/>
@@ -1802,8 +1790,8 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="14">
-        <f>SUM(B1,D1,G2)</f>
-        <v>0.14850694444444443</v>
+        <f>SUM(B1,D1,G1,J2:J5)</f>
+        <v>0.28503472222222215</v>
       </c>
       <c r="I20" s="8">
         <v>8.6030092592592589E-2</v>
@@ -1863,8 +1851,8 @@
         <v>43784</v>
       </c>
       <c r="C24" s="2">
-        <f>SUM(G2:G9)</f>
-        <v>6.3182870370370375E-2</v>
+        <f>SUM(G2:G12)</f>
+        <v>8.924768518518518E-2</v>
       </c>
       <c r="I24" s="10">
         <v>6.7789351851851851E-2</v>
@@ -1875,12 +1863,12 @@
       <c r="X24" s="1"/>
     </row>
     <row r="25" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>134</v>
+      <c r="B25" s="15">
+        <v>43785</v>
       </c>
       <c r="C25" s="2">
-        <f>G1-C24</f>
-        <v>3.6643518518518506E-2</v>
+        <f>SUM(G13,J2:J5)</f>
+        <v>4.9548611111111106E-2</v>
       </c>
       <c r="I25" s="10">
         <v>5.5787037037037031E-2</v>

</xml_diff>

<commit_message>
finished chapter 6 OOP Book List Project with persisting in local storage
</commit_message>
<xml_diff>
--- a/videos_Lengths.xlsx
+++ b/videos_Lengths.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="135">
   <si>
     <t>Chapter 2 : JavaScript Language Fundamentals</t>
   </si>
@@ -418,13 +419,16 @@
   </si>
   <si>
     <t>total completed time so far</t>
+  </si>
+  <si>
+    <t>total to completed time so far</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,8 +496,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF336600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF336600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF336600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,6 +555,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -544,7 +576,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -553,7 +585,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="46" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="21" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="46" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="46" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -565,6 +596,16 @@
     <xf numFmtId="21" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="46" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="1" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
@@ -575,11 +616,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FF66"/>
+      <color rgb="FF66FF33"/>
       <color rgb="FF336600"/>
-      <color rgb="FF66FF66"/>
       <color rgb="FF339933"/>
       <color rgb="FF008000"/>
-      <color rgb="FF66FF33"/>
     </mruColors>
   </colors>
   <extLst>
@@ -892,20 +933,20 @@
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
     <col min="17" max="17" width="2.28515625" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
     <col min="20" max="20" width="3.7109375" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" customWidth="1"/>
     <col min="23" max="23" width="2.5703125" customWidth="1"/>
     <col min="24" max="24" width="8.7109375" customWidth="1"/>
     <col min="26" max="26" width="2.42578125" customWidth="1"/>
-    <col min="27" max="27" width="9.5703125" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" customWidth="1"/>
     <col min="29" max="29" width="3.85546875" customWidth="1"/>
     <col min="30" max="30" width="9.28515625" customWidth="1"/>
     <col min="32" max="32" width="2.28515625" customWidth="1"/>
@@ -1008,40 +1049,40 @@
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="28">
         <v>3.9467592592592592E-3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="28">
         <v>3.0208333333333333E-3</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <v>2.2685185185185182E-3</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="18">
         <v>1.1030092592592591E-2</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="11">
         <v>8.2870370370370372E-3</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="28">
         <v>5.7870370370370376E-3</v>
       </c>
       <c r="R2" t="s">
@@ -1088,40 +1129,40 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="28">
         <v>1.4930555555555556E-3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="28">
         <v>6.2615740740740748E-3</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="16">
         <v>1.0636574074074074E-2</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="18">
         <v>9.7685185185185184E-3</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="11">
         <v>8.518518518518519E-3</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="28">
         <v>8.7037037037037031E-3</v>
       </c>
       <c r="R3" t="s">
@@ -1168,40 +1209,40 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="28">
         <v>7.0023148148148154E-3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="28">
         <v>8.8541666666666664E-3</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>9.8726851851851857E-3</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="18">
         <v>7.6736111111111111E-3</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="28">
         <v>6.875E-3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="28">
         <v>5.8796296296296296E-3</v>
       </c>
       <c r="R4" t="s">
@@ -1248,34 +1289,34 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="28">
         <v>7.1759259259259259E-3</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="16">
         <v>1.0023148148148147E-2</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="18">
         <v>1.0497685185185186E-2</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="28">
         <v>5.8333333333333336E-3</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="28">
         <v>4.5138888888888893E-3</v>
       </c>
       <c r="R5" t="s">
@@ -1322,34 +1363,34 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="28">
         <v>8.1365740740740738E-3</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <v>1.0983796296296297E-2</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="11">
         <v>1.1655092592592594E-2</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="28">
         <v>3.8078703703703707E-3</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="28">
         <v>4.2361111111111106E-3</v>
       </c>
       <c r="R6" t="s">
@@ -1396,34 +1437,34 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="28">
         <v>5.0810185185185186E-3</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>4.7106481481481478E-3</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="11">
         <v>4.386574074074074E-3</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="28">
         <v>5.9606481481481489E-3</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="28">
         <v>1.0231481481481482E-2</v>
       </c>
       <c r="R7" t="s">
@@ -1470,28 +1511,28 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="28">
         <v>9.9652777777777778E-3</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <v>7.6041666666666662E-3</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="11">
         <v>4.8726851851851856E-3</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="28">
         <v>4.0162037037037033E-3</v>
       </c>
       <c r="R8" t="s">
@@ -1526,22 +1567,22 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="28">
         <v>7.0254629629629634E-3</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>7.083333333333333E-3</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="11">
         <v>1.1469907407407408E-2</v>
       </c>
       <c r="R9" t="s">
@@ -1570,22 +1611,22 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="28">
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="15">
         <v>7.6851851851851847E-3</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="11">
         <v>7.1180555555555554E-3</v>
       </c>
       <c r="R10" t="s">
@@ -1611,19 +1652,19 @@
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>5.4398148148148149E-3</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <v>8.8310185185185176E-3</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="11">
         <v>7.5578703703703702E-3</v>
       </c>
       <c r="R11" t="s">
@@ -1644,13 +1685,13 @@
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>6.4120370370370364E-3</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="15">
         <v>9.5486111111111101E-3</v>
       </c>
       <c r="R12" t="s">
@@ -1670,13 +1711,13 @@
       <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>1.3217592592592593E-2</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>1.0578703703703703E-2</v>
       </c>
       <c r="R13" t="s">
@@ -1696,7 +1737,7 @@
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>3.3449074074074071E-3</v>
       </c>
       <c r="R14" t="s">
@@ -1710,7 +1751,7 @@
       <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>8.1481481481481474E-3</v>
       </c>
       <c r="R15" t="s">
@@ -1724,7 +1765,7 @@
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>1.1585648148148149E-2</v>
       </c>
       <c r="R16" t="s">
@@ -1738,39 +1779,63 @@
       <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>1.4479166666666668E-2</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="19">
         <v>1.2442129629629629E-2</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="20" t="s">
         <v>128</v>
       </c>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <v>4.5370370370370365E-3</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="22">
         <v>0.1337962962962963</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="20" t="s">
         <v>0</v>
       </c>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I19" s="10">
+      <c r="I19" s="22">
         <v>9.9826388888888895E-2</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="20" t="s">
         <v>18</v>
       </c>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="7"/>
@@ -1783,40 +1848,69 @@
       <c r="AF19" s="6"/>
     </row>
     <row r="20" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14">
-        <f>SUM(B1,D1,G1,J2:J5)</f>
-        <v>0.28503472222222215</v>
-      </c>
-      <c r="I20" s="8">
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13">
+        <f>SUM(B1,D1,G1,J1,M1,P1)</f>
+        <v>0.41474537037037035</v>
+      </c>
+      <c r="I20" s="19">
         <v>8.6030092592592589E-2</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="20" t="s">
         <v>31</v>
       </c>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I21" s="10">
+      <c r="C21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
+        <f>I32-G20</f>
+        <v>0.50329861111111129</v>
+      </c>
+      <c r="I21" s="19">
         <v>4.3298611111111107E-2</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="20" t="s">
         <v>42</v>
       </c>
+      <c r="K21" s="19"/>
+      <c r="L21" s="20"/>
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I22" s="10">
+      <c r="B22" s="14">
+        <v>43783</v>
+      </c>
+      <c r="C22" s="11">
+        <f>SUM(D11:D18,G2)</f>
+        <v>6.9432870370370367E-2</v>
+      </c>
+      <c r="I22" s="19">
         <v>3.9351851851851853E-2</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J22" s="20" t="s">
         <v>50</v>
       </c>
+      <c r="K22" s="19"/>
+      <c r="L22" s="20"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="7"/>
@@ -1831,114 +1925,121 @@
       <c r="AF22" s="6"/>
     </row>
     <row r="23" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" s="15">
-        <v>43783</v>
-      </c>
-      <c r="C23" s="2">
-        <f>SUM(D11:D18,G2)</f>
-        <v>6.9432870370370367E-2</v>
-      </c>
-      <c r="I23" s="10">
+      <c r="B23" s="25">
+        <v>43784</v>
+      </c>
+      <c r="C23" s="26">
+        <f>SUM(G3:G12)</f>
+        <v>8.6979166666666663E-2</v>
+      </c>
+      <c r="I23" s="9">
         <v>0.10527777777777779</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="J23" s="8" t="s">
         <v>57</v>
       </c>
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="15">
-        <v>43784</v>
-      </c>
-      <c r="C24" s="2">
-        <f>SUM(G2:G12)</f>
-        <v>8.924768518518518E-2</v>
-      </c>
-      <c r="I24" s="10">
-        <v>6.7789351851851851E-2</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="X24" s="1"/>
-    </row>
-    <row r="25" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="15">
+      <c r="B24" s="23">
         <v>43785</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C24" s="24">
         <f>SUM(G13,J2:J5)</f>
         <v>4.9548611111111106E-2</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I24" s="9">
+        <v>6.7789351851851851E-2</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="14">
+        <v>43786</v>
+      </c>
+      <c r="C25" s="11">
+        <f>SUM(J6:J11,M2:M3)</f>
+        <v>6.3865740740740751E-2</v>
+      </c>
+      <c r="I25" s="9">
         <v>5.5787037037037031E-2</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="8" t="s">
         <v>83</v>
       </c>
       <c r="U25" s="6"/>
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I26" s="10">
+      <c r="B26" s="14">
+        <v>43787</v>
+      </c>
+      <c r="C26" s="28">
+        <f>SUM(M4:M8,P1)</f>
+        <v>6.5844907407407408E-2</v>
+      </c>
+      <c r="I26" s="9">
         <v>6.0428240740740741E-2</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="8" t="s">
         <v>90</v>
       </c>
       <c r="U26" s="6"/>
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I27" s="10">
+      <c r="I27" s="9">
         <v>4.5717592592592594E-2</v>
       </c>
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="8" t="s">
         <v>97</v>
       </c>
       <c r="U27" s="7"/>
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I28" s="10">
+      <c r="I28" s="9">
         <v>0.10824074074074075</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="8" t="s">
         <v>105</v>
       </c>
       <c r="U28" s="6"/>
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I29" s="10">
+      <c r="I29" s="9">
         <v>5.8541666666666665E-2</v>
       </c>
-      <c r="J29" s="9" t="s">
+      <c r="J29" s="8" t="s">
         <v>118</v>
       </c>
       <c r="U29" s="6"/>
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I30" s="10">
+      <c r="I30" s="9">
         <v>1.5162037037037036E-3</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="8" t="s">
         <v>127</v>
       </c>
       <c r="U30" s="6"/>
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
       <c r="U31" s="6"/>
     </row>
     <row r="32" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>132</v>
       </c>
-      <c r="H32" s="11"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="3">
         <f>SUM(I17:I30)</f>
         <v>0.91804398148148159</v>

</xml_diff>

<commit_message>
finished chapter 8 part 1
</commit_message>
<xml_diff>
--- a/videos_Lengths.xlsx
+++ b/videos_Lengths.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="137">
   <si>
     <t>Chapter 2 : JavaScript Language Fundamentals</t>
   </si>
@@ -422,6 +421,12 @@
   </si>
   <si>
     <t>total to completed time so far</t>
+  </si>
+  <si>
+    <t>Github Finder</t>
+  </si>
+  <si>
+    <t>WeatherJS</t>
   </si>
 </sst>
 </file>
@@ -921,7 +926,7 @@
   <dimension ref="A1:AK36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1014,7 @@
         <v>73</v>
       </c>
       <c r="V1" s="6">
-        <f xml:space="preserve"> SUM(V2:V18)</f>
+        <f xml:space="preserve"> SUM(V2:V10)</f>
         <v>6.7789351851851851E-2</v>
       </c>
       <c r="X1" s="5" t="s">
@@ -1085,16 +1090,16 @@
       <c r="P2" s="28">
         <v>5.7870370370370376E-3</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="11">
         <v>2.5578703703703705E-3</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="11">
         <v>9.5486111111111101E-3</v>
       </c>
       <c r="X2" t="s">
@@ -1165,10 +1170,10 @@
       <c r="P3" s="28">
         <v>8.7037037037037031E-3</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="11">
         <v>4.1666666666666666E-3</v>
       </c>
       <c r="U3" t="s">
@@ -1245,10 +1250,10 @@
       <c r="P4" s="28">
         <v>5.8796296296296296E-3</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="11">
         <v>8.9120370370370378E-3</v>
       </c>
       <c r="U4" t="s">
@@ -1319,10 +1324,10 @@
       <c r="P5" s="28">
         <v>4.5138888888888893E-3</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="11">
         <v>0.01</v>
       </c>
       <c r="U5" t="s">
@@ -1393,10 +1398,10 @@
       <c r="P6" s="28">
         <v>4.2361111111111106E-3</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="11">
         <v>1.0381944444444444E-2</v>
       </c>
       <c r="U6" t="s">
@@ -1467,10 +1472,10 @@
       <c r="P7" s="28">
         <v>1.0231481481481482E-2</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="11">
         <v>4.5601851851851853E-3</v>
       </c>
       <c r="U7" t="s">
@@ -1535,10 +1540,10 @@
       <c r="M8" s="28">
         <v>4.0162037037037033E-3</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="11">
         <v>5.8796296296296296E-3</v>
       </c>
       <c r="U8" t="s">
@@ -1585,10 +1590,10 @@
       <c r="J9" s="11">
         <v>1.1469907407407408E-2</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="11">
         <v>1.0717592592592593E-2</v>
       </c>
       <c r="U9" t="s">
@@ -1629,10 +1634,10 @@
       <c r="J10" s="11">
         <v>7.1180555555555554E-3</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="11">
         <v>8.4837962962962966E-3</v>
       </c>
       <c r="U10" t="s">
@@ -1667,10 +1672,10 @@
       <c r="J11" s="11">
         <v>7.5578703703703702E-3</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="11">
         <v>3.9236111111111112E-3</v>
       </c>
       <c r="Z11" s="2"/>
@@ -1694,11 +1699,14 @@
       <c r="G12" s="15">
         <v>9.5486111111111101E-3</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="11">
         <v>8.7962962962962968E-3</v>
+      </c>
+      <c r="V12" s="6">
+        <v>6.7789351851851851E-2</v>
       </c>
       <c r="AG12" t="s">
         <v>116</v>
@@ -1720,10 +1728,10 @@
       <c r="G13" s="18">
         <v>1.0578703703703703E-2</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" s="11">
         <v>8.4490740740740741E-3</v>
       </c>
       <c r="AG13" t="s">
@@ -1740,10 +1748,10 @@
       <c r="D14" s="11">
         <v>3.3449074074074071E-3</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="11">
         <v>8.9699074074074073E-3</v>
       </c>
     </row>
@@ -1754,11 +1762,18 @@
       <c r="D15" s="11">
         <v>8.1481481481481474E-3</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" s="11">
         <v>5.6134259259259271E-3</v>
+      </c>
+      <c r="U15" t="s">
+        <v>135</v>
+      </c>
+      <c r="V15" s="2">
+        <f>SUM(V2:V6)</f>
+        <v>3.9143518518518515E-2</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -1768,11 +1783,18 @@
       <c r="D16" s="11">
         <v>1.1585648148148149E-2</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16" s="11">
         <v>3.8657407407407408E-3</v>
+      </c>
+      <c r="U16" t="s">
+        <v>136</v>
+      </c>
+      <c r="V16" s="2">
+        <f>V12-V15</f>
+        <v>2.8645833333333336E-2</v>
       </c>
     </row>
     <row r="17" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
@@ -1855,8 +1877,8 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="13">
-        <f>SUM(B1,D1,G1,J1,M1,P1)</f>
-        <v>0.41474537037037035</v>
+        <f>SUM(B1,D1,G1,J1,M1,P1,S1,V2)</f>
+        <v>0.52957175925925926</v>
       </c>
       <c r="I20" s="19">
         <v>8.6030092592592589E-2</v>
@@ -1883,7 +1905,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3">
         <f>I32-G20</f>
-        <v>0.50329861111111129</v>
+        <v>0.38847222222222233</v>
       </c>
       <c r="I21" s="19">
         <v>4.3298611111111107E-2</v>
@@ -1991,6 +2013,13 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" s="14">
+        <v>43788</v>
+      </c>
+      <c r="C27" s="2">
+        <f>SUM(S1,V2)</f>
+        <v>0.11482638888888889</v>
+      </c>
       <c r="I27" s="9">
         <v>4.5717592592592594E-2</v>
       </c>

</xml_diff>